<commit_message>
Add geographic_location column to airports table
</commit_message>
<xml_diff>
--- a/data/Airports.xlsx
+++ b/data/Airports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysiek\Documents\GitHub\flight_db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D5EB8-280A-4618-8834-4A277DFFDE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3F373F-A2AA-488A-BC22-7E593D8389D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D641D20-2ABD-40C9-9F29-9BF9A7988FB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="334">
   <si>
     <t>PDL</t>
   </si>
@@ -1027,6 +1027,15 @@
   </si>
   <si>
     <t>Minneapolis Saint Paul International Airport</t>
+  </si>
+  <si>
+    <t>geographic_location</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>North America</t>
   </si>
 </sst>
 </file>
@@ -1391,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD80715E-5489-4D96-ABF9-FD4C8D3849C6}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1415,7 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>315</v>
       </c>
@@ -1422,8 +1431,13 @@
       <c r="E1" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1439,8 +1453,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1456,8 +1473,11 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1473,8 +1493,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1490,8 +1513,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1507,8 +1533,11 @@
       <c r="E6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1524,8 +1553,11 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1541,8 +1573,11 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1558,8 +1593,11 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1575,8 +1613,11 @@
       <c r="E10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1592,8 +1633,11 @@
       <c r="E11" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1609,8 +1653,11 @@
       <c r="E12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1626,8 +1673,11 @@
       <c r="E13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1643,8 +1693,11 @@
       <c r="E14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1660,8 +1713,11 @@
       <c r="E15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1677,8 +1733,11 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1694,8 +1753,11 @@
       <c r="E17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1711,8 +1773,11 @@
       <c r="E18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1728,8 +1793,11 @@
       <c r="E19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1745,8 +1813,11 @@
       <c r="E20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1762,8 +1833,11 @@
       <c r="E21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1779,8 +1853,11 @@
       <c r="E22" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1796,8 +1873,11 @@
       <c r="E23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1813,8 +1893,11 @@
       <c r="E24" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1830,8 +1913,11 @@
       <c r="E25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1847,8 +1933,11 @@
       <c r="E26" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1864,8 +1953,11 @@
       <c r="E27" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1881,8 +1973,11 @@
       <c r="E28" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1898,8 +1993,11 @@
       <c r="E29" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1915,8 +2013,11 @@
       <c r="E30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1932,8 +2033,11 @@
       <c r="E31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1949,8 +2053,11 @@
       <c r="E32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1966,8 +2073,11 @@
       <c r="E33" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1983,8 +2093,11 @@
       <c r="E34" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2000,8 +2113,11 @@
       <c r="E35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2017,8 +2133,11 @@
       <c r="E36" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2034,8 +2153,11 @@
       <c r="E37" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2051,8 +2173,11 @@
       <c r="E38" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2068,8 +2193,11 @@
       <c r="E39" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2085,8 +2213,11 @@
       <c r="E40" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2102,8 +2233,11 @@
       <c r="E41" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2119,8 +2253,11 @@
       <c r="E42" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2136,8 +2273,11 @@
       <c r="E43" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2153,8 +2293,11 @@
       <c r="E44" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2170,8 +2313,11 @@
       <c r="E45" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2187,8 +2333,11 @@
       <c r="E46" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2204,8 +2353,11 @@
       <c r="E47" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2221,8 +2373,11 @@
       <c r="E48" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2238,8 +2393,11 @@
       <c r="E49" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2255,8 +2413,11 @@
       <c r="E50" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2272,8 +2433,11 @@
       <c r="E51" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2289,8 +2453,11 @@
       <c r="E52" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2306,8 +2473,11 @@
       <c r="E53" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2323,8 +2493,11 @@
       <c r="E54" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2340,8 +2513,11 @@
       <c r="E55" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2357,8 +2533,11 @@
       <c r="E56" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2374,8 +2553,11 @@
       <c r="E57" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2391,8 +2573,11 @@
       <c r="E58" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2408,8 +2593,11 @@
       <c r="E59" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2425,8 +2613,11 @@
       <c r="E60" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2442,8 +2633,11 @@
       <c r="E61" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2459,8 +2653,11 @@
       <c r="E62" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2476,8 +2673,11 @@
       <c r="E63" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2493,8 +2693,11 @@
       <c r="E64" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2510,8 +2713,11 @@
       <c r="E65" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2527,8 +2733,11 @@
       <c r="E66" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2544,8 +2753,11 @@
       <c r="E67" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2561,8 +2773,11 @@
       <c r="E68" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2578,8 +2793,11 @@
       <c r="E69" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2595,8 +2813,11 @@
       <c r="E70" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2612,8 +2833,11 @@
       <c r="E71" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2629,8 +2853,11 @@
       <c r="E72" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2646,8 +2873,11 @@
       <c r="E73" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2663,8 +2893,11 @@
       <c r="E74" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2680,8 +2913,11 @@
       <c r="E75" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2697,8 +2933,11 @@
       <c r="E76" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2714,8 +2953,11 @@
       <c r="E77" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2731,8 +2973,11 @@
       <c r="E78" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2748,8 +2993,11 @@
       <c r="E79" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2765,8 +3013,11 @@
       <c r="E80" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2782,8 +3033,11 @@
       <c r="E81" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2799,8 +3053,11 @@
       <c r="E82" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2816,8 +3073,11 @@
       <c r="E83" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2833,8 +3093,11 @@
       <c r="E84" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2850,8 +3113,11 @@
       <c r="E85" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2867,8 +3133,11 @@
       <c r="E86" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2884,8 +3153,11 @@
       <c r="E87" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2901,8 +3173,11 @@
       <c r="E88" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2918,8 +3193,11 @@
       <c r="E89" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2935,8 +3213,11 @@
       <c r="E90" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2952,8 +3233,11 @@
       <c r="E91" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2969,8 +3253,11 @@
       <c r="E92" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2986,8 +3273,11 @@
       <c r="E93" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3003,8 +3293,11 @@
       <c r="E94" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3020,8 +3313,11 @@
       <c r="E95" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3037,8 +3333,11 @@
       <c r="E96" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3054,8 +3353,11 @@
       <c r="E97" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3071,8 +3373,11 @@
       <c r="E98" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3088,8 +3393,11 @@
       <c r="E99" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3105,8 +3413,11 @@
       <c r="E100" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3122,8 +3433,11 @@
       <c r="E101" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3138,6 +3452,9 @@
       </c>
       <c r="E102" t="s">
         <v>253</v>
+      </c>
+      <c r="F102" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>